<commit_message>
Update LBO example with balanced Sources & Uses
- Generated with fixed Sources & Uses calculation
- CHECK now shows $0 (balanced)
- Uses real data from Financial_Model_Data_Source.xlsx
- LTM EBITDA: $663M, Entry Multiple: 8.5x
- Total Uses: $5,748M properly balanced with Sources
</commit_message>
<xml_diff>
--- a/Examples/LBO_Model_AcmeTech.xlsx
+++ b/Examples/LBO_Model_AcmeTech.xlsx
@@ -849,7 +849,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sponsor Equity (% of Purchase Price)</t>
+          <t>Sponsor Equity (% of Total Uses)</t>
         </is>
       </c>
       <c r="B44" s="11" t="n">
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="B45" s="7">
-        <f>B13*B44</f>
+        <f>B27*B44</f>
         <v/>
       </c>
     </row>
@@ -897,7 +897,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Senior Debt (% of Purchase Price)</t>
+          <t>Senior Debt (% of Total Uses)</t>
         </is>
       </c>
       <c r="B50" s="11" t="n">
@@ -911,7 +911,7 @@
         </is>
       </c>
       <c r="B51" s="7">
-        <f>B13*B50</f>
+        <f>B27*B50</f>
         <v/>
       </c>
     </row>
@@ -938,7 +938,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Subordinated Debt (% of Purchase Price)</t>
+          <t>Subordinated Debt (% of Total Uses)</t>
         </is>
       </c>
       <c r="B54" s="11" t="n">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B55" s="7">
-        <f>B13*B54</f>
+        <f>B27*B54</f>
         <v/>
       </c>
     </row>

</xml_diff>